<commit_message>
Added support to read variables from Config file
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\UiPath\TnPAutomation\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22CA5A6A-FC3E-43B5-A8AE-DC8744FADB49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B01AE4EF-ADF1-40F7-8DCB-1F4DC30045B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2544" yWindow="2544" windowWidth="19572" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2688" yWindow="2688" windowWidth="19572" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="57">
   <si>
     <t>Name</t>
   </si>
@@ -162,22 +162,40 @@
     <t>ProcessABCQueue</t>
   </si>
   <si>
-    <t>inputGR</t>
-  </si>
-  <si>
     <t>inputStudentMaster</t>
   </si>
   <si>
-    <t>Data\Input\StudentData.xlsx</t>
-  </si>
-  <si>
-    <t>Data\Input\GRnumbers.xlsx</t>
-  </si>
-  <si>
     <t>inputSheet</t>
   </si>
   <si>
     <t>Sheet1</t>
+  </si>
+  <si>
+    <t>D:\Downloads\UiPath\TnPAutomation\Data\Input\Companies\</t>
+  </si>
+  <si>
+    <t>inputCompanyFile</t>
+  </si>
+  <si>
+    <t>D:\Downloads\UiPath\TnPAutomation\Data\Input\StudentData.xlsx</t>
+  </si>
+  <si>
+    <t>companyUrl</t>
+  </si>
+  <si>
+    <t>https://firebasestorage.googleapis.com/v0/b/eazytnp-8a32c.appspot.com/o/Registrations%2F</t>
+  </si>
+  <si>
+    <t>studentDbUrl</t>
+  </si>
+  <si>
+    <t>https://firebasestorage.googleapis.com/v0/b/eazytnp-8a32c.appspot.com/o/StudentData.xlsx</t>
+  </si>
+  <si>
+    <t>entryUrl</t>
+  </si>
+  <si>
+    <t>https://firestore.googleapis.com/v1/projects/eazytnp-8a32c/databases/(default)/documents/Company</t>
   </si>
 </sst>
 </file>
@@ -554,16 +572,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z999"/>
+  <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="43.5546875" customWidth="1"/>
-    <col min="2" max="2" width="43" customWidth="1"/>
+    <col min="2" max="2" width="86.44140625" customWidth="1"/>
     <col min="3" max="3" width="81.44140625" customWidth="1"/>
     <col min="4" max="26" width="8.6640625" customWidth="1"/>
   </cols>
@@ -636,15 +654,15 @@
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" s="2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>50</v>
@@ -652,15 +670,36 @@
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>47</v>
+        <v>49</v>
+      </c>
+      <c r="B8" t="s">
+        <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A9" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B9" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A10" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B10" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A11" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B11" t="s">
+        <v>56</v>
+      </c>
+    </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1648,7 +1687,6 @@
     <row r="996" ht="14.25" customHeight="1"/>
     <row r="997" ht="14.25" customHeight="1"/>
     <row r="998" ht="14.25" customHeight="1"/>
-    <row r="999" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
T&P Automation BOT version 1.0.1 Release
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\UiPath\TnPAutomation\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBDA8979-A213-4A0A-B5FB-C6849E7E6233}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD26AAC9-7ABF-41E4-8999-C67A769223B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1428" yWindow="1428" windowWidth="19572" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3024" yWindow="2760" windowWidth="19572" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="71">
   <si>
     <t>Name</t>
   </si>
@@ -232,6 +232,12 @@
   </si>
   <si>
     <t>Placed Students</t>
+  </si>
+  <si>
+    <t>https://firestore.googleapis.com/v1beta1/projects/eazytnp-8a32c/databases/(default)/documents/Company/</t>
+  </si>
+  <si>
+    <t>processedUrl</t>
   </si>
 </sst>
 </file>
@@ -608,10 +614,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z998"/>
+  <dimension ref="A1:Z999"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -738,53 +744,60 @@
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>57</v>
+        <v>70</v>
+      </c>
+      <c r="B12" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" s="2" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="B14" t="s">
-        <v>62</v>
+        <v>58</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>64</v>
+        <v>61</v>
+      </c>
+      <c r="B15" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
       <c r="A16" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="14.25" customHeight="1">
       <c r="A17" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A18" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B18" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="19" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="20" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="21" spans="1:2" ht="14.25" customHeight="1"/>
@@ -1765,6 +1778,7 @@
     <row r="996" ht="14.25" customHeight="1"/>
     <row r="997" ht="14.25" customHeight="1"/>
     <row r="998" ht="14.25" customHeight="1"/>
+    <row r="999" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>